<commit_message>
Bug fix - amend sim scripts accordingly
</commit_message>
<xml_diff>
--- a/Fig5/Make Pop Model/Switching time estimation results.xlsx
+++ b/Fig5/Make Pop Model/Switching time estimation results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ersat\CODE\punisher\Fig5\Make Pop Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA4709E-11BB-45F7-A43D-D3F2CE57D6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FE798F-2B8B-43CE-8936-551619AB82C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{7EBF1748-0CF1-4662-A168-45D48256CF16}"/>
   </bookViews>
   <sheets>
-    <sheet name="New values" sheetId="4" r:id="rId1"/>
-    <sheet name="Old values" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Newest values" sheetId="5" r:id="rId1"/>
+    <sheet name="New values" sheetId="4" r:id="rId2"/>
+    <sheet name="Old values" sheetId="1" r:id="rId3"/>
+    <sheet name="Definition" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="79">
   <si>
     <t>Genetic state</t>
   </si>
@@ -266,13 +266,16 @@
     <t>Same as OSOC:L (OSPC:H)</t>
   </si>
   <si>
-    <t>Can't see :/</t>
-  </si>
-  <si>
     <t>Based on binomial distribution instead</t>
   </si>
   <si>
     <t>See artificial</t>
+  </si>
+  <si>
+    <t>Absolute confint</t>
+  </si>
+  <si>
+    <t>Nope</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1081,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1235,12 +1238,17 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="14" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="23" xfId="14" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="26" xfId="14" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="14" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="14" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="15" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="14" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1253,61 +1261,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="50" xfId="16" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="16" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="16" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="19" xfId="16" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="16" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="16" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="16" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="19" xfId="16" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1330,7 +1338,37 @@
     <cellStyle name="Output" xfId="5" builtinId="21"/>
     <cellStyle name="Style 1" xfId="16" xr:uid="{B3F15202-CEAB-4127-B01E-2003158D3113}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1720,10 +1758,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F521E6-BB43-4468-83BF-3DFBB1030687}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1ADE348-E800-4392-A3DF-091F8BCCF346}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1740,10 +1778,11 @@
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="42.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1778,11 +1817,694 @@
         <v>30</v>
       </c>
       <c r="L1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="16">
+        <v>10.505928691524</v>
+      </c>
+      <c r="G2" s="17">
+        <v>10.355733734600101</v>
+      </c>
+      <c r="H2" s="24">
+        <v>10.6591945597328</v>
+      </c>
+      <c r="I2" s="31">
+        <f>(H2-G2)/F2</f>
+        <v>2.8884721574164714E-2</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2">
+        <f>(H2-G2)</f>
+        <v>0.30346082513269934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="114"/>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="13">
+        <v>10</v>
+      </c>
+      <c r="E3" s="108" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="18">
+        <v>1549.39876665112</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="36">
+        <v>30000</v>
+      </c>
+      <c r="D4" s="33">
+        <v>10</v>
+      </c>
+      <c r="E4" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5.3146353293626696</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5.2499772246384904</v>
+      </c>
+      <c r="H4" s="26">
+        <v>5.3806276320752797</v>
+      </c>
+      <c r="I4" s="29">
+        <f t="shared" ref="I4:I17" si="0">(H4-G4)/F4</f>
+        <v>2.4583136817490154E-2</v>
+      </c>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L17" si="1">(H4-G4)</f>
+        <v>0.13065040743678935</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="116"/>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="22">
+        <v>37494.9997777522</v>
+      </c>
+      <c r="G5" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="16">
+        <v>2.5889613333333301</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2.5596739183227499</v>
+      </c>
+      <c r="H6" s="24">
+        <v>2.6188979630104101</v>
+      </c>
+      <c r="I6" s="31">
+        <f t="shared" si="0"/>
+        <v>2.287560031319906E-2</v>
+      </c>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>5.9224044687660182E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="114"/>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="14">
+        <v>4.8999999999999897</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1.4883150822976099</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1.47133534013778</v>
+      </c>
+      <c r="H7" s="25">
+        <v>1.5056655493173401</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="0"/>
+        <v>2.3066492833333577E-2</v>
+      </c>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>3.4330209179560089E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D8" s="10">
+        <v>10</v>
+      </c>
+      <c r="E8" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="20">
+        <v>2.3950883333333302</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2.3680736220797902</v>
+      </c>
+      <c r="H8" s="26">
+        <v>2.42270572821409</v>
+      </c>
+      <c r="I8" s="29">
+        <f t="shared" si="0"/>
+        <v>2.2810058975263909E-2</v>
+      </c>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8">
+        <f>(H8-G8)</f>
+        <v>5.4632106134299807E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="116"/>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>5.62</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1.2672792179628301</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1.2530113935312299</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1.2818667646669399</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="0"/>
+        <v>2.2769544964286126E-2</v>
+      </c>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9">
+        <f>(H9-G9)</f>
+        <v>2.8855371135710017E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="111" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3.0482563333333301</v>
+      </c>
+      <c r="G10" s="17">
+        <v>3.0134716214035202</v>
+      </c>
+      <c r="H10" s="17">
+        <v>3.0838002359191798</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="0"/>
+        <v>2.3071752118285233E-2</v>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10">
+        <f>(H10-G10)</f>
+        <v>7.0328614515659638E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
+      <c r="B11" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="44">
+        <v>30000</v>
+      </c>
+      <c r="D11" s="45">
+        <v>10</v>
+      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
+      <c r="L11">
+        <f>(H11-G11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="10">
+        <v>10</v>
+      </c>
+      <c r="E12" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="20">
+        <v>2.6326089999999902</v>
+      </c>
+      <c r="G12" s="21">
+        <v>2.6028062108072398</v>
+      </c>
+      <c r="H12" s="21">
+        <v>2.6630714584066499</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="0"/>
+        <v>2.2891833766203157E-2</v>
+      </c>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>6.0265247599410099E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="116"/>
+      <c r="B13" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="44">
+        <v>30000</v>
+      </c>
+      <c r="D13" s="45">
+        <v>10</v>
+      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="41"/>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2.6935069999999999</v>
+      </c>
+      <c r="G14" s="17">
+        <v>2.66298277658621</v>
+      </c>
+      <c r="H14" s="60">
+        <v>2.7247054714924999</v>
+      </c>
+      <c r="I14" s="66">
+        <f t="shared" si="0"/>
+        <v>2.2915364580931068E-2</v>
+      </c>
+      <c r="J14" s="104"/>
+      <c r="K14" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>6.1722694906289899E-2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="114"/>
+      <c r="B15" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="14">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1.48431226266088</v>
+      </c>
+      <c r="G15" s="19">
+        <v>1.4673698377117099</v>
+      </c>
+      <c r="H15" s="57">
+        <v>1.5016243124297599</v>
+      </c>
+      <c r="I15" s="67">
+        <f t="shared" si="0"/>
+        <v>2.3077674138892491E-2</v>
+      </c>
+      <c r="J15" s="105"/>
+      <c r="K15" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>3.4254474718049988E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10</v>
+      </c>
+      <c r="E16" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="20">
+        <v>2.4581770000000001</v>
+      </c>
+      <c r="G16" s="21">
+        <v>2.4304255954148801</v>
+      </c>
+      <c r="H16" s="58">
+        <v>2.4865462510969198</v>
+      </c>
+      <c r="I16" s="62">
+        <f t="shared" si="0"/>
+        <v>2.2830193139891767E-2</v>
+      </c>
+      <c r="J16" s="104"/>
+      <c r="K16" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>5.6120655682039722E-2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="116"/>
+      <c r="B17" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D17" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.62</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1.26634012879116</v>
+      </c>
+      <c r="G17" s="23">
+        <v>1.2520831656881</v>
+      </c>
+      <c r="H17" s="59">
+        <v>1.2809165872436199</v>
+      </c>
+      <c r="I17" s="63">
+        <f t="shared" si="0"/>
+        <v>2.2769097259078514E-2</v>
+      </c>
+      <c r="J17" s="106"/>
+      <c r="K17" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>2.8833421555519934E-2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I17">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F521E6-BB43-4468-83BF-3DFBB1030687}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="47.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="113" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1814,9 +2536,13 @@
       <c r="K2" s="47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="109"/>
+      <c r="L2">
+        <f>(H2-G2)</f>
+        <v>0.33597535696759984</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="114"/>
       <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
@@ -1845,12 +2571,12 @@
       <c r="K3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="L3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="110" t="s">
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="115" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1882,9 +2608,13 @@
       <c r="K4" s="49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="111"/>
+      <c r="L4">
+        <f t="shared" ref="L4:L17" si="1">(H4-G4)</f>
+        <v>0.13959539751365035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="116"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1913,12 +2643,12 @@
       <c r="K5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="L5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="108" t="s">
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="113" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1950,17 +2680,21 @@
       <c r="K6" s="47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="109"/>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>5.9518739642340002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="114"/>
       <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="15">
         <v>30000</v>
       </c>
-      <c r="D7" s="103" t="s">
-        <v>77</v>
+      <c r="D7" s="102" t="s">
+        <v>76</v>
       </c>
       <c r="E7" s="14">
         <v>4.8999999999999897</v>
@@ -1982,9 +2716,13 @@
       <c r="K7" s="48" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="110" t="s">
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>3.4429600932589954E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="115" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2016,20 +2754,24 @@
       <c r="K8" s="49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111"/>
+      <c r="L8">
+        <f>(H8-G8)</f>
+        <v>5.490211005841017E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="116"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="8">
         <v>30000</v>
       </c>
-      <c r="D9" s="104" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>75</v>
+      <c r="D9" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>6.9</v>
       </c>
       <c r="F9" s="22">
         <v>1.2701454739581499</v>
@@ -2048,9 +2790,13 @@
       <c r="K9" s="50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="108" t="s">
+      <c r="L9">
+        <f>(H9-G9)</f>
+        <v>2.8922376668669925E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="113" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -2082,12 +2828,16 @@
       <c r="K10" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <f>(H10-G10)</f>
+        <v>7.2347586334910119E-2</v>
+      </c>
+      <c r="M10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="109"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
       <c r="B11" s="42"/>
       <c r="C11" s="44"/>
       <c r="D11" s="45"/>
@@ -2098,12 +2848,16 @@
       <c r="I11" s="38"/>
       <c r="J11" s="39"/>
       <c r="K11" s="40"/>
-      <c r="L11" t="s">
+      <c r="L11">
+        <f>(H11-G11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="110" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="115" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
@@ -2135,12 +2889,16 @@
       <c r="K12" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>6.2064888485759973E-2</v>
+      </c>
+      <c r="M12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="111"/>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="116"/>
       <c r="B13" s="42"/>
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
@@ -2151,12 +2909,16 @@
       <c r="I13" s="65"/>
       <c r="J13" s="61"/>
       <c r="K13" s="41"/>
-      <c r="L13" t="s">
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="108" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="34" t="s">
@@ -2168,7 +2930,7 @@
       <c r="D14" s="1">
         <v>10</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="16">
@@ -2184,26 +2946,30 @@
         <f t="shared" si="0"/>
         <v>2.2920974311777604E-2</v>
       </c>
-      <c r="J14" s="105"/>
+      <c r="J14" s="104"/>
       <c r="K14" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>6.2061968454959704E-2</v>
+      </c>
+      <c r="M14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="109"/>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="114"/>
       <c r="B15" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="15">
         <v>30000</v>
       </c>
-      <c r="D15" s="103" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="13">
+      <c r="D15" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="14">
         <v>4.8499999999999996</v>
       </c>
       <c r="F15" s="18">
@@ -2219,16 +2985,20 @@
         <f t="shared" si="0"/>
         <v>2.308050753928588E-2</v>
       </c>
-      <c r="J15" s="106"/>
+      <c r="J15" s="105"/>
       <c r="K15" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>3.4323640693119994E-2</v>
+      </c>
+      <c r="M15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="110" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="115" t="s">
         <v>21</v>
       </c>
       <c r="B16" t="s">
@@ -2240,7 +3010,7 @@
       <c r="D16" s="10">
         <v>10</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="20">
@@ -2256,27 +3026,31 @@
         <f t="shared" si="0"/>
         <v>2.2834244451753458E-2</v>
       </c>
-      <c r="J16" s="105"/>
+      <c r="J16" s="104"/>
       <c r="K16" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>5.6410821148760171E-2</v>
+      </c>
+      <c r="M16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111"/>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="116"/>
       <c r="B17" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="8">
         <v>30000</v>
       </c>
-      <c r="D17" s="104" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="102" t="s">
-        <v>75</v>
+      <c r="D17" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.62</v>
       </c>
       <c r="F17" s="22">
         <v>1.2685709042375699</v>
@@ -2291,11 +3065,15 @@
         <f t="shared" si="0"/>
         <v>2.2770162135037103E-2</v>
       </c>
-      <c r="J17" s="107"/>
+      <c r="J17" s="106"/>
       <c r="K17" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>2.8885565169280092E-2</v>
+      </c>
+      <c r="M17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2329,7 +3107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A3A4DA-47DF-46FC-8995-3BB85B702A4F}">
   <dimension ref="A1:M17"/>
   <sheetViews>
@@ -2392,7 +3170,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="113" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2428,7 +3206,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="109"/>
+      <c r="A3" s="114"/>
       <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
@@ -2468,7 +3246,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="115" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -2504,7 +3282,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="111"/>
+      <c r="A5" s="116"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2534,7 +3312,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="113" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2570,7 +3348,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="109"/>
+      <c r="A7" s="114"/>
       <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
@@ -2604,7 +3382,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="115" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2640,7 +3418,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111"/>
+      <c r="A9" s="116"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2674,7 +3452,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="113" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -2713,7 +3491,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="109"/>
+      <c r="A11" s="114"/>
       <c r="B11" s="42"/>
       <c r="C11" s="44"/>
       <c r="D11" s="45"/>
@@ -2729,7 +3507,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="115" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
@@ -2768,7 +3546,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="111"/>
+      <c r="A13" s="116"/>
       <c r="B13" s="42"/>
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
@@ -2784,7 +3562,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="108" t="s">
+      <c r="A14" s="113" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="34" t="s">
@@ -2817,7 +3595,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="109"/>
+      <c r="A15" s="114"/>
       <c r="B15" s="43" t="s">
         <v>9</v>
       </c>
@@ -2848,7 +3626,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="110" t="s">
+      <c r="A16" s="115" t="s">
         <v>21</v>
       </c>
       <c r="B16" t="s">
@@ -2881,7 +3659,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111"/>
+      <c r="A17" s="116"/>
       <c r="B17" s="35" t="s">
         <v>9</v>
       </c>
@@ -2941,24 +3719,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D929F84-4E66-4E15-A743-8460A0034F9D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21DB94-5D85-43CF-BB32-E65D083B0EA7}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C31"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,7 +3754,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="129" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3005,7 +3771,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="120"/>
+      <c r="A3" s="130"/>
       <c r="B3" s="14" t="s">
         <v>36</v>
       </c>
@@ -3020,7 +3786,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="125" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -3037,7 +3803,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="122"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -3052,7 +3818,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="127" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -3069,7 +3835,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="126"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="11" t="s">
         <v>36</v>
       </c>
@@ -3084,7 +3850,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
+      <c r="A8" s="128"/>
       <c r="B8" s="14">
         <v>0</v>
       </c>
@@ -3099,7 +3865,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="128" t="s">
+      <c r="A9" s="123" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -3116,7 +3882,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="126"/>
+      <c r="A10" s="120"/>
       <c r="B10" s="11" t="s">
         <v>36</v>
       </c>
@@ -3131,7 +3897,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="129"/>
+      <c r="A11" s="124"/>
       <c r="B11" s="14">
         <v>0</v>
       </c>
@@ -3146,7 +3912,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="121" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -3163,7 +3929,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="118"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="14" t="s">
         <v>36</v>
       </c>
@@ -3178,7 +3944,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="123" t="s">
+      <c r="A14" s="117" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -3195,7 +3961,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+      <c r="A15" s="119"/>
       <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
@@ -3210,7 +3976,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="125" t="s">
+      <c r="A16" s="127" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -3227,7 +3993,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="126"/>
+      <c r="A17" s="120"/>
       <c r="B17" s="11" t="s">
         <v>36</v>
       </c>
@@ -3242,7 +4008,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="127"/>
+      <c r="A18" s="128"/>
       <c r="B18" s="14">
         <v>0</v>
       </c>
@@ -3257,7 +4023,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="128" t="s">
+      <c r="A19" s="123" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3274,7 +4040,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="126"/>
+      <c r="A20" s="120"/>
       <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
@@ -3289,7 +4055,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="129"/>
+      <c r="A21" s="124"/>
       <c r="B21" s="14">
         <v>0</v>
       </c>
@@ -3304,230 +4070,264 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="117" t="s">
+      <c r="C22" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="117" t="s">
+      <c r="D22" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="115" t="s">
+      <c r="E22" s="133" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="120"/>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="116"/>
+      <c r="A23" s="130"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="134"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="125" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="123" t="s">
+      <c r="B24" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="112">
+      <c r="D24" s="131">
         <v>0</v>
       </c>
-      <c r="E24" s="112" t="s">
+      <c r="E24" s="131" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="122"/>
-      <c r="B25" s="124"/>
-      <c r="C25" s="124"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
+      <c r="A25" s="126"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="125" t="s">
+      <c r="A26" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="117" t="s">
+      <c r="C26" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="126" t="s">
+      <c r="D26" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="115" t="s">
+      <c r="E26" s="133" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="126"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="130"/>
-      <c r="D27" s="126"/>
-      <c r="E27" s="113"/>
+      <c r="A27" s="120"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="135"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="127"/>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="116"/>
+      <c r="A28" s="128"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="122"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="134"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="128" t="s">
+      <c r="A29" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="123" t="s">
+      <c r="B29" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="123" t="s">
+      <c r="C29" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="112">
+      <c r="D29" s="131">
         <v>0</v>
       </c>
-      <c r="E29" s="112" t="s">
+      <c r="E29" s="131" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="126"/>
-      <c r="B30" s="130"/>
-      <c r="C30" s="130"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="113"/>
+      <c r="A30" s="120"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="135"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="129"/>
-      <c r="B31" s="124"/>
-      <c r="C31" s="124"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
+      <c r="A31" s="124"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="117" t="s">
+      <c r="B32" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="117" t="s">
+      <c r="C32" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="117" t="s">
+      <c r="D32" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="115" t="s">
+      <c r="E32" s="133" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="118"/>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="116"/>
+      <c r="A33" s="122"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="134"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="123" t="s">
+      <c r="B34" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="123" t="s">
+      <c r="C34" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="112">
+      <c r="D34" s="131">
         <v>0</v>
       </c>
-      <c r="E34" s="112" t="s">
+      <c r="E34" s="131" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="124"/>
-      <c r="B35" s="124"/>
-      <c r="C35" s="124"/>
-      <c r="D35" s="114"/>
-      <c r="E35" s="114"/>
+      <c r="A35" s="119"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="132"/>
+      <c r="E35" s="132"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="125" t="s">
+      <c r="A36" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="117" t="s">
+      <c r="B36" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="117" t="s">
+      <c r="C36" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="117" t="s">
+      <c r="D36" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="115" t="s">
+      <c r="E36" s="133" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="126"/>
-      <c r="B37" s="130"/>
-      <c r="C37" s="130"/>
-      <c r="D37" s="130"/>
-      <c r="E37" s="113"/>
+      <c r="A37" s="120"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="118"/>
+      <c r="D37" s="118"/>
+      <c r="E37" s="135"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="127"/>
-      <c r="B38" s="118"/>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="116"/>
+      <c r="A38" s="128"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="122"/>
+      <c r="D38" s="122"/>
+      <c r="E38" s="134"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="128" t="s">
+      <c r="A39" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="123" t="s">
+      <c r="B39" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="112">
+      <c r="D39" s="131">
         <v>0</v>
       </c>
-      <c r="E39" s="112" t="s">
+      <c r="E39" s="131" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="126"/>
-      <c r="B40" s="130"/>
-      <c r="C40" s="130"/>
-      <c r="D40" s="113"/>
-      <c r="E40" s="113"/>
+      <c r="A40" s="120"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="135"/>
+      <c r="E40" s="135"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="129"/>
-      <c r="B41" s="124"/>
-      <c r="C41" s="124"/>
-      <c r="D41" s="114"/>
-      <c r="E41" s="114"/>
+      <c r="A41" s="124"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="132"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E42" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A38"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="D32:D33"/>
@@ -3542,40 +4342,6 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C36:C38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D29:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tidy up non-program files
</commit_message>
<xml_diff>
--- a/Fig5/Make Pop Model/Switching time estimation results.xlsx
+++ b/Fig5/Make Pop Model/Switching time estimation results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ersat\CODE\punisher\Fig5\Make Pop Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FE798F-2B8B-43CE-8936-551619AB82C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463279F9-E0BE-4FF3-8BB1-38ED4B333856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{7EBF1748-0CF1-4662-A168-45D48256CF16}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{7EBF1748-0CF1-4662-A168-45D48256CF16}"/>
   </bookViews>
   <sheets>
-    <sheet name="Newest values" sheetId="5" r:id="rId1"/>
-    <sheet name="New values" sheetId="4" r:id="rId2"/>
-    <sheet name="Old values" sheetId="1" r:id="rId3"/>
-    <sheet name="Definition" sheetId="2" r:id="rId4"/>
+    <sheet name="Newest values after peer review" sheetId="6" r:id="rId1"/>
+    <sheet name="Newer values" sheetId="5" r:id="rId2"/>
+    <sheet name="New values" sheetId="4" r:id="rId3"/>
+    <sheet name="Old values" sheetId="1" r:id="rId4"/>
+    <sheet name="Definition" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="79">
   <si>
     <t>Genetic state</t>
   </si>
@@ -1261,49 +1262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="50" xfId="16" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="50" xfId="16" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="16" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="16" applyBorder="1">
@@ -1315,7 +1277,46 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="19" xfId="16" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="16" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1338,7 +1339,37 @@
     <cellStyle name="Output" xfId="5" builtinId="21"/>
     <cellStyle name="Style 1" xfId="16" xr:uid="{B3F15202-CEAB-4127-B01E-2003158D3113}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1758,11 +1789,672 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB7912F-77BB-4E31-8260-6CDEDCC067BE}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="16">
+        <v>10.5062352882998</v>
+      </c>
+      <c r="G2" s="17">
+        <v>10.3560346394676</v>
+      </c>
+      <c r="H2" s="24">
+        <v>10.6595069706113</v>
+      </c>
+      <c r="I2" s="31">
+        <f>(H2-G2)/F2</f>
+        <v>2.8884973809948856E-2</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L17" si="0">(H2-G2)</f>
+        <v>0.3034723311437002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="114"/>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="13">
+        <v>10</v>
+      </c>
+      <c r="E3" s="108" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="18">
+        <v>1541.3863461926701</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="36">
+        <v>30000</v>
+      </c>
+      <c r="D4" s="33">
+        <v>10</v>
+      </c>
+      <c r="E4" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5.3145634807417901</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5.2499063986182897</v>
+      </c>
+      <c r="H4" s="26">
+        <v>5.3805547411946097</v>
+      </c>
+      <c r="I4" s="29">
+        <f t="shared" ref="I4:I17" si="1">(H4-G4)/F4</f>
+        <v>2.4583080633008941E-2</v>
+      </c>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0.13064834257632008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="116"/>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="22">
+        <v>37494.9997777522</v>
+      </c>
+      <c r="G5" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="16">
+        <v>2.5890123333333301</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2.55972431695325</v>
+      </c>
+      <c r="H6" s="24">
+        <v>2.6189495765987898</v>
+      </c>
+      <c r="I6" s="31">
+        <f t="shared" si="1"/>
+        <v>2.2875618969836205E-2</v>
+      </c>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>5.9225259645539818E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="114"/>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="14">
+        <v>4.8999999999999897</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1.48828081961706</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1.4713014935969699</v>
+      </c>
+      <c r="H7" s="25">
+        <v>1.5056308622797001</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="1"/>
+        <v>2.3066459118624701E-2</v>
+      </c>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>3.4329368682730177E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D8" s="10">
+        <v>10</v>
+      </c>
+      <c r="E8" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="20">
+        <v>2.3951579999999999</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2.3681424767201</v>
+      </c>
+      <c r="H8" s="26">
+        <v>2.4227762236646901</v>
+      </c>
+      <c r="I8" s="29">
+        <f t="shared" si="1"/>
+        <v>2.2810080564451329E-2</v>
+      </c>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>5.4633746944590111E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="116"/>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>5.62</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1.2672535281753501</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1.25298600087975</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1.2818407715359399</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="1"/>
+        <v>2.2769532705690182E-2</v>
+      </c>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>2.885477065618991E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="111" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3.0482069999999899</v>
+      </c>
+      <c r="G10" s="17">
+        <v>3.0134228877023501</v>
+      </c>
+      <c r="H10" s="17">
+        <v>3.0837502911196299</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="1"/>
+        <v>2.307172820523018E-2</v>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>7.0327403417279832E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
+      <c r="B11" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="44">
+        <v>30000</v>
+      </c>
+      <c r="D11" s="45">
+        <v>10</v>
+      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="10">
+        <v>10</v>
+      </c>
+      <c r="E12" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="20">
+        <v>2.63274266666666</v>
+      </c>
+      <c r="G12" s="21">
+        <v>2.6029382970254602</v>
+      </c>
+      <c r="H12" s="21">
+        <v>2.6632067375298498</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="1"/>
+        <v>2.2891884295207648E-2</v>
+      </c>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>6.026844050438962E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="116"/>
+      <c r="B13" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="44">
+        <v>30000</v>
+      </c>
+      <c r="D13" s="45">
+        <v>10</v>
+      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="41"/>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2.6936049999999998</v>
+      </c>
+      <c r="G14" s="17">
+        <v>2.6630796133599199</v>
+      </c>
+      <c r="H14" s="60">
+        <v>2.7248046581745702</v>
+      </c>
+      <c r="I14" s="66">
+        <f t="shared" si="1"/>
+        <v>2.2915403266124859E-2</v>
+      </c>
+      <c r="J14" s="104"/>
+      <c r="K14" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>6.1725044814650243E-2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="114"/>
+      <c r="B15" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="14">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1.4843136068824101</v>
+      </c>
+      <c r="G15" s="19">
+        <v>1.4673711655808199</v>
+      </c>
+      <c r="H15" s="57">
+        <v>1.5016256733262301</v>
+      </c>
+      <c r="I15" s="67">
+        <f t="shared" si="1"/>
+        <v>2.3077675490260373E-2</v>
+      </c>
+      <c r="J15" s="105"/>
+      <c r="K15" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>3.4254507745410168E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10</v>
+      </c>
+      <c r="E16" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="20">
+        <v>2.4582609999999998</v>
+      </c>
+      <c r="G16" s="21">
+        <v>2.4305086127298599</v>
+      </c>
+      <c r="H16" s="58">
+        <v>2.4866312539551099</v>
+      </c>
+      <c r="I16" s="62">
+        <f t="shared" si="1"/>
+        <v>2.2830220723206372E-2</v>
+      </c>
+      <c r="J16" s="104"/>
+      <c r="K16" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>5.6122641225250014E-2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="116"/>
+      <c r="B17" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D17" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.62</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1.2663297854592701</v>
+      </c>
+      <c r="G17" s="23">
+        <v>1.2520729419799099</v>
+      </c>
+      <c r="H17" s="59">
+        <v>1.28090612178857</v>
+      </c>
+      <c r="I17" s="63">
+        <f t="shared" si="1"/>
+        <v>2.2769092332612952E-2</v>
+      </c>
+      <c r="J17" s="106"/>
+      <c r="K17" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>2.883317980866007E-2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1ADE348-E800-4392-A3DF-091F8BCCF346}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,6 +3094,676 @@
       <c r="L17">
         <f t="shared" si="1"/>
         <v>2.8833421555519934E-2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I17">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F521E6-BB43-4468-83BF-3DFBB1030687}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="47.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="16">
+        <v>11.357780722265501</v>
+      </c>
+      <c r="G2" s="17">
+        <v>11.191502831813301</v>
+      </c>
+      <c r="H2" s="24">
+        <v>11.527478188780901</v>
+      </c>
+      <c r="I2" s="31">
+        <f>(H2-G2)/F2</f>
+        <v>2.9581074435515595E-2</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2">
+        <f>(H2-G2)</f>
+        <v>0.33597535696759984</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="114"/>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="13">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="18">
+        <v>1153.2939326298299</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="36">
+        <v>30000</v>
+      </c>
+      <c r="D4" s="33">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5.6228050282567699</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5.5537170948119501</v>
+      </c>
+      <c r="H4" s="26">
+        <v>5.6933124923256004</v>
+      </c>
+      <c r="I4" s="29">
+        <f t="shared" ref="I4:I17" si="0">(H4-G4)/F4</f>
+        <v>2.4826647342763887E-2</v>
+      </c>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L17" si="1">(H4-G4)</f>
+        <v>0.13959539751365035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="116"/>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="22">
+        <v>29994.9997221792</v>
+      </c>
+      <c r="G5" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="16">
+        <v>2.6013269999999999</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2.57189371871221</v>
+      </c>
+      <c r="H6" s="24">
+        <v>2.63141245835455</v>
+      </c>
+      <c r="I6" s="31">
+        <f t="shared" si="0"/>
+        <v>2.2880145265220406E-2</v>
+      </c>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>5.9518739642340002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="114"/>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="14">
+        <v>4.8999999999999897</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1.49236560946109</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1.4753366571867901</v>
+      </c>
+      <c r="H7" s="25">
+        <v>1.50976625811938</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="0"/>
+        <v>2.3070486691945998E-2</v>
+      </c>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>3.4429600932589954E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D8" s="10">
+        <v>10</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="20">
+        <v>2.40654866666666</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2.3794003315678398</v>
+      </c>
+      <c r="H8" s="26">
+        <v>2.43430244162625</v>
+      </c>
+      <c r="I8" s="29">
+        <f t="shared" si="0"/>
+        <v>2.2813629667608491E-2</v>
+      </c>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8">
+        <f>(H8-G8)</f>
+        <v>5.490211005841017E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="116"/>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>6.9</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1.2701454739581499</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1.2558444930201</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1.28476686968877</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="0"/>
+        <v>2.2770916608897736E-2</v>
+      </c>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9">
+        <f>(H9-G9)</f>
+        <v>2.8922376668669925E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3.1302656666666602</v>
+      </c>
+      <c r="G10" s="17">
+        <v>3.0944813128791</v>
+      </c>
+      <c r="H10" s="17">
+        <v>3.1668288992140101</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="0"/>
+        <v>2.311228312194703E-2</v>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10">
+        <f>(H10-G10)</f>
+        <v>7.2347586334910119E-2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
+      <c r="L11">
+        <f>(H11-G11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="10">
+        <v>10</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="20">
+        <v>2.70777133333333</v>
+      </c>
+      <c r="G12" s="21">
+        <v>2.6770777201083602</v>
+      </c>
+      <c r="H12" s="21">
+        <v>2.7391426085941202</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="0"/>
+        <v>2.2921022806366976E-2</v>
+      </c>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>6.2064888485759973E-2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="116"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="41"/>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2.7076496666666601</v>
+      </c>
+      <c r="G14" s="17">
+        <v>2.6769574988980702</v>
+      </c>
+      <c r="H14" s="60">
+        <v>2.7390194673530299</v>
+      </c>
+      <c r="I14" s="66">
+        <f t="shared" si="0"/>
+        <v>2.2920974311777604E-2</v>
+      </c>
+      <c r="J14" s="104"/>
+      <c r="K14" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>6.2061968454959704E-2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="114"/>
+      <c r="B15" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="15">
+        <v>30000</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="14">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1.4871267728708699</v>
+      </c>
+      <c r="G15" s="19">
+        <v>1.47015010259936</v>
+      </c>
+      <c r="H15" s="57">
+        <v>1.50447374329248</v>
+      </c>
+      <c r="I15" s="67">
+        <f t="shared" si="0"/>
+        <v>2.308050753928588E-2</v>
+      </c>
+      <c r="J15" s="105"/>
+      <c r="K15" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>3.4323640693119994E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="20">
+        <v>2.47044833333333</v>
+      </c>
+      <c r="G16" s="21">
+        <v>2.44255331933274</v>
+      </c>
+      <c r="H16" s="58">
+        <v>2.4989641404815002</v>
+      </c>
+      <c r="I16" s="62">
+        <f t="shared" si="0"/>
+        <v>2.2834244451753458E-2</v>
+      </c>
+      <c r="J16" s="104"/>
+      <c r="K16" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>5.6410821148760171E-2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="116"/>
+      <c r="B17" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8">
+        <v>30000</v>
+      </c>
+      <c r="D17" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.62</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1.2685709042375699</v>
+      </c>
+      <c r="G17" s="23">
+        <v>1.25428813884032</v>
+      </c>
+      <c r="H17" s="59">
+        <v>1.2831737040096001</v>
+      </c>
+      <c r="I17" s="63">
+        <f t="shared" si="0"/>
+        <v>2.2770162135037103E-2</v>
+      </c>
+      <c r="J17" s="106"/>
+      <c r="K17" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>2.8885565169280092E-2</v>
       </c>
       <c r="M17" t="s">
         <v>28</v>
@@ -2437,677 +3799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F521E6-BB43-4468-83BF-3DFBB1030687}">
-  <dimension ref="A1:M17"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="47.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7">
-        <v>30000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="16">
-        <v>11.357780722265501</v>
-      </c>
-      <c r="G2" s="17">
-        <v>11.191502831813301</v>
-      </c>
-      <c r="H2" s="24">
-        <v>11.527478188780901</v>
-      </c>
-      <c r="I2" s="31">
-        <f>(H2-G2)/F2</f>
-        <v>2.9581074435515595E-2</v>
-      </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2">
-        <f>(H2-G2)</f>
-        <v>0.33597535696759984</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="114"/>
-      <c r="B3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="15">
-        <v>30000</v>
-      </c>
-      <c r="D3" s="13">
-        <v>10</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="18">
-        <v>1153.2939326298299</v>
-      </c>
-      <c r="G3" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="97" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="98" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="115" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="36">
-        <v>30000</v>
-      </c>
-      <c r="D4" s="33">
-        <v>10</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="20">
-        <v>5.6228050282567699</v>
-      </c>
-      <c r="G4" s="21">
-        <v>5.5537170948119501</v>
-      </c>
-      <c r="H4" s="26">
-        <v>5.6933124923256004</v>
-      </c>
-      <c r="I4" s="29">
-        <f t="shared" ref="I4:I17" si="0">(H4-G4)/F4</f>
-        <v>2.4826647342763887E-2</v>
-      </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L17" si="1">(H4-G4)</f>
-        <v>0.13959539751365035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="116"/>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8">
-        <v>30000</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="22">
-        <v>29994.9997221792</v>
-      </c>
-      <c r="G5" s="99" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="113" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7">
-        <v>30000</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="16">
-        <v>2.6013269999999999</v>
-      </c>
-      <c r="G6" s="17">
-        <v>2.57189371871221</v>
-      </c>
-      <c r="H6" s="24">
-        <v>2.63141245835455</v>
-      </c>
-      <c r="I6" s="31">
-        <f t="shared" si="0"/>
-        <v>2.2880145265220406E-2</v>
-      </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>5.9518739642340002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="15">
-        <v>30000</v>
-      </c>
-      <c r="D7" s="102" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="14">
-        <v>4.8999999999999897</v>
-      </c>
-      <c r="F7" s="18">
-        <v>1.49236560946109</v>
-      </c>
-      <c r="G7" s="19">
-        <v>1.4753366571867901</v>
-      </c>
-      <c r="H7" s="25">
-        <v>1.50976625811938</v>
-      </c>
-      <c r="I7" s="32">
-        <f t="shared" si="0"/>
-        <v>2.3070486691945998E-2</v>
-      </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
-        <v>3.4429600932589954E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="115" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12">
-        <v>30000</v>
-      </c>
-      <c r="D8" s="10">
-        <v>10</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="20">
-        <v>2.40654866666666</v>
-      </c>
-      <c r="G8" s="21">
-        <v>2.3794003315678398</v>
-      </c>
-      <c r="H8" s="26">
-        <v>2.43430244162625</v>
-      </c>
-      <c r="I8" s="29">
-        <f t="shared" si="0"/>
-        <v>2.2813629667608491E-2</v>
-      </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8">
-        <f>(H8-G8)</f>
-        <v>5.490211005841017E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="116"/>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="8">
-        <v>30000</v>
-      </c>
-      <c r="D9" s="103" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9">
-        <v>6.9</v>
-      </c>
-      <c r="F9" s="22">
-        <v>1.2701454739581499</v>
-      </c>
-      <c r="G9" s="23">
-        <v>1.2558444930201</v>
-      </c>
-      <c r="H9" s="27">
-        <v>1.28476686968877</v>
-      </c>
-      <c r="I9" s="30">
-        <f t="shared" si="0"/>
-        <v>2.2770916608897736E-2</v>
-      </c>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9">
-        <f>(H9-G9)</f>
-        <v>2.8922376668669925E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="113" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7">
-        <v>30000</v>
-      </c>
-      <c r="D10" s="1">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="16">
-        <v>3.1302656666666602</v>
-      </c>
-      <c r="G10" s="17">
-        <v>3.0944813128791</v>
-      </c>
-      <c r="H10" s="17">
-        <v>3.1668288992140101</v>
-      </c>
-      <c r="I10" s="30">
-        <f t="shared" si="0"/>
-        <v>2.311228312194703E-2</v>
-      </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10">
-        <f>(H10-G10)</f>
-        <v>7.2347586334910119E-2</v>
-      </c>
-      <c r="M10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="114"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
-      <c r="L11">
-        <f>(H11-G11)</f>
-        <v>0</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="115" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="12">
-        <v>30000</v>
-      </c>
-      <c r="D12" s="10">
-        <v>10</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="20">
-        <v>2.70777133333333</v>
-      </c>
-      <c r="G12" s="21">
-        <v>2.6770777201083602</v>
-      </c>
-      <c r="H12" s="21">
-        <v>2.7391426085941202</v>
-      </c>
-      <c r="I12" s="29">
-        <f t="shared" si="0"/>
-        <v>2.2921022806366976E-2</v>
-      </c>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
-        <v>6.2064888485759973E-2</v>
-      </c>
-      <c r="M12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="41"/>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="113" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="7">
-        <v>30000</v>
-      </c>
-      <c r="D14" s="1">
-        <v>10</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="16">
-        <v>2.7076496666666601</v>
-      </c>
-      <c r="G14" s="17">
-        <v>2.6769574988980702</v>
-      </c>
-      <c r="H14" s="60">
-        <v>2.7390194673530299</v>
-      </c>
-      <c r="I14" s="66">
-        <f t="shared" si="0"/>
-        <v>2.2920974311777604E-2</v>
-      </c>
-      <c r="J14" s="104"/>
-      <c r="K14" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>6.2061968454959704E-2</v>
-      </c>
-      <c r="M14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
-      <c r="B15" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="15">
-        <v>30000</v>
-      </c>
-      <c r="D15" s="102" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="14">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="F15" s="18">
-        <v>1.4871267728708699</v>
-      </c>
-      <c r="G15" s="19">
-        <v>1.47015010259936</v>
-      </c>
-      <c r="H15" s="57">
-        <v>1.50447374329248</v>
-      </c>
-      <c r="I15" s="67">
-        <f t="shared" si="0"/>
-        <v>2.308050753928588E-2</v>
-      </c>
-      <c r="J15" s="105"/>
-      <c r="K15" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
-        <v>3.4323640693119994E-2</v>
-      </c>
-      <c r="M15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="115" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="12">
-        <v>30000</v>
-      </c>
-      <c r="D16" s="10">
-        <v>10</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="20">
-        <v>2.47044833333333</v>
-      </c>
-      <c r="G16" s="21">
-        <v>2.44255331933274</v>
-      </c>
-      <c r="H16" s="58">
-        <v>2.4989641404815002</v>
-      </c>
-      <c r="I16" s="62">
-        <f t="shared" si="0"/>
-        <v>2.2834244451753458E-2</v>
-      </c>
-      <c r="J16" s="104"/>
-      <c r="K16" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
-        <v>5.6410821148760171E-2</v>
-      </c>
-      <c r="M16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="116"/>
-      <c r="B17" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="8">
-        <v>30000</v>
-      </c>
-      <c r="D17" s="103" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="5">
-        <v>5.62</v>
-      </c>
-      <c r="F17" s="22">
-        <v>1.2685709042375699</v>
-      </c>
-      <c r="G17" s="23">
-        <v>1.25428813884032</v>
-      </c>
-      <c r="H17" s="59">
-        <v>1.2831737040096001</v>
-      </c>
-      <c r="I17" s="63">
-        <f t="shared" si="0"/>
-        <v>2.2770162135037103E-2</v>
-      </c>
-      <c r="J17" s="106"/>
-      <c r="K17" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>2.8885565169280092E-2</v>
-      </c>
-      <c r="M17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-  </mergeCells>
-  <conditionalFormatting sqref="I2:I10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I17">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A3A4DA-47DF-46FC-8995-3BB85B702A4F}">
   <dimension ref="A1:M17"/>
   <sheetViews>
@@ -3701,17 +4393,17 @@
     <mergeCell ref="A10:A11"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:I17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3719,7 +4411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21DB94-5D85-43CF-BB32-E65D083B0EA7}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -3754,7 +4446,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="124" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3771,7 +4463,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="130"/>
+      <c r="A3" s="125"/>
       <c r="B3" s="14" t="s">
         <v>36</v>
       </c>
@@ -3786,7 +4478,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="126" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -3803,7 +4495,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -3818,7 +4510,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="127" t="s">
+      <c r="A6" s="130" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -3835,7 +4527,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="120"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="11" t="s">
         <v>36</v>
       </c>
@@ -3850,7 +4542,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
+      <c r="A8" s="132"/>
       <c r="B8" s="14">
         <v>0</v>
       </c>
@@ -3865,7 +4557,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="133" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -3882,7 +4574,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="120"/>
+      <c r="A10" s="131"/>
       <c r="B10" s="11" t="s">
         <v>36</v>
       </c>
@@ -3897,7 +4589,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="134"/>
       <c r="B11" s="14">
         <v>0</v>
       </c>
@@ -3912,7 +4604,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="122" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -3929,7 +4621,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="14" t="s">
         <v>36</v>
       </c>
@@ -3944,7 +4636,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="128" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -3961,7 +4653,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="119"/>
+      <c r="A15" s="129"/>
       <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
@@ -3976,7 +4668,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="127" t="s">
+      <c r="A16" s="130" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -3993,7 +4685,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="120"/>
+      <c r="A17" s="131"/>
       <c r="B17" s="11" t="s">
         <v>36</v>
       </c>
@@ -4008,7 +4700,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="128"/>
+      <c r="A18" s="132"/>
       <c r="B18" s="14">
         <v>0</v>
       </c>
@@ -4023,7 +4715,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="123" t="s">
+      <c r="A19" s="133" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -4040,7 +4732,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="120"/>
+      <c r="A20" s="131"/>
       <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
@@ -4055,7 +4747,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="124"/>
+      <c r="A21" s="134"/>
       <c r="B21" s="14">
         <v>0</v>
       </c>
@@ -4070,264 +4762,230 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="129" t="s">
+      <c r="A22" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="121" t="s">
+      <c r="B22" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="121" t="s">
+      <c r="C22" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="121" t="s">
+      <c r="D22" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="133" t="s">
+      <c r="E22" s="120" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="130"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
-      <c r="E23" s="134"/>
+      <c r="A23" s="125"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="121"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="125" t="s">
+      <c r="A24" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="117" t="s">
+      <c r="C24" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="131">
+      <c r="D24" s="117">
         <v>0</v>
       </c>
-      <c r="E24" s="131" t="s">
+      <c r="E24" s="117" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="126"/>
-      <c r="B25" s="119"/>
-      <c r="C25" s="119"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
+      <c r="A25" s="127"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="127" t="s">
+      <c r="A26" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="121" t="s">
+      <c r="B26" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="121" t="s">
+      <c r="C26" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="120" t="s">
+      <c r="D26" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="133" t="s">
+      <c r="E26" s="120" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="120"/>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="135"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="118"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="128"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="122"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="134"/>
+      <c r="A28" s="132"/>
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="121"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="117" t="s">
+      <c r="B29" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="117" t="s">
+      <c r="C29" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="131">
+      <c r="D29" s="117">
         <v>0</v>
       </c>
-      <c r="E29" s="131" t="s">
+      <c r="E29" s="117" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="120"/>
-      <c r="B30" s="118"/>
-      <c r="C30" s="118"/>
-      <c r="D30" s="135"/>
-      <c r="E30" s="135"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="135"/>
+      <c r="C30" s="135"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="118"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="124"/>
-      <c r="B31" s="119"/>
-      <c r="C31" s="119"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
+      <c r="A31" s="134"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="119"/>
+      <c r="E31" s="119"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="121" t="s">
+      <c r="A32" s="122" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="121" t="s">
+      <c r="B32" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="121" t="s">
+      <c r="C32" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="121" t="s">
+      <c r="D32" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="133" t="s">
+      <c r="E32" s="120" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="122"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="122"/>
-      <c r="D33" s="122"/>
-      <c r="E33" s="134"/>
+      <c r="A33" s="123"/>
+      <c r="B33" s="123"/>
+      <c r="C33" s="123"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="121"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="117" t="s">
+      <c r="A34" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="117" t="s">
+      <c r="B34" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="117" t="s">
+      <c r="C34" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="131">
+      <c r="D34" s="117">
         <v>0</v>
       </c>
-      <c r="E34" s="131" t="s">
+      <c r="E34" s="117" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="119"/>
-      <c r="B35" s="119"/>
-      <c r="C35" s="119"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="132"/>
+      <c r="A35" s="129"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="119"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="127" t="s">
+      <c r="A36" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="121" t="s">
+      <c r="B36" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="121" t="s">
+      <c r="C36" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="121" t="s">
+      <c r="D36" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="133" t="s">
+      <c r="E36" s="120" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
-      <c r="B37" s="118"/>
-      <c r="C37" s="118"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="135"/>
+      <c r="A37" s="131"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="118"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="128"/>
-      <c r="B38" s="122"/>
-      <c r="C38" s="122"/>
-      <c r="D38" s="122"/>
-      <c r="E38" s="134"/>
+      <c r="A38" s="132"/>
+      <c r="B38" s="123"/>
+      <c r="C38" s="123"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="121"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="123" t="s">
+      <c r="A39" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="117" t="s">
+      <c r="B39" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="117" t="s">
+      <c r="C39" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="131">
+      <c r="D39" s="117">
         <v>0</v>
       </c>
-      <c r="E39" s="131" t="s">
+      <c r="E39" s="117" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
-      <c r="B40" s="118"/>
-      <c r="C40" s="118"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
+      <c r="A40" s="131"/>
+      <c r="B40" s="135"/>
+      <c r="C40" s="135"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="124"/>
-      <c r="B41" s="119"/>
-      <c r="C41" s="119"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="132"/>
+      <c r="A41" s="134"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="119"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E42" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A38"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="D32:D33"/>
@@ -4342,6 +5000,40 @@
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D29:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>